<commit_message>
Fix mô hình As, update banner
</commit_message>
<xml_diff>
--- a/admin/pages/Association-Rules/dataset/viewlist.xlsx
+++ b/admin/pages/Association-Rules/dataset/viewlist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>ngayxem</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>2024-06-22</t>
+  </si>
+  <si>
+    <t>2024-06-23</t>
+  </si>
+  <si>
+    <t>2024-06-26</t>
+  </si>
+  <si>
+    <t>2024-06-27</t>
+  </si>
+  <si>
+    <t>2024-06-28</t>
+  </si>
+  <si>
+    <t>2024-06-29</t>
   </si>
 </sst>
 </file>
@@ -425,7 +440,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C793"/>
+  <dimension ref="A1:C872"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -9154,6 +9169,875 @@
       </c>
       <c r="C793" s="0">
         <v>61</v>
+      </c>
+    </row>
+    <row r="794" spans="1:3">
+      <c r="A794" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B794" s="0">
+        <v>49</v>
+      </c>
+      <c r="C794" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="795" spans="1:3">
+      <c r="A795" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B795" s="0">
+        <v>49</v>
+      </c>
+      <c r="C795" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="796" spans="1:3">
+      <c r="A796" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B796" s="0">
+        <v>49</v>
+      </c>
+      <c r="C796" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="797" spans="1:3">
+      <c r="A797" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B797" s="0">
+        <v>49</v>
+      </c>
+      <c r="C797" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="798" spans="1:3">
+      <c r="A798" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B798" s="0">
+        <v>49</v>
+      </c>
+      <c r="C798" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="799" spans="1:3">
+      <c r="A799" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B799" s="0">
+        <v>49</v>
+      </c>
+      <c r="C799" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="800" spans="1:3">
+      <c r="A800" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B800" s="0">
+        <v>49</v>
+      </c>
+      <c r="C800" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3">
+      <c r="A801" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B801" s="0">
+        <v>49</v>
+      </c>
+      <c r="C801" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="802" spans="1:3">
+      <c r="A802" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B802" s="0">
+        <v>49</v>
+      </c>
+      <c r="C802" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="803" spans="1:3">
+      <c r="A803" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B803" s="0">
+        <v>49</v>
+      </c>
+      <c r="C803" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="804" spans="1:3">
+      <c r="A804" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B804" s="0">
+        <v>49</v>
+      </c>
+      <c r="C804" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="805" spans="1:3">
+      <c r="A805" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B805" s="0">
+        <v>49</v>
+      </c>
+      <c r="C805" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3">
+      <c r="A806" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B806" s="0">
+        <v>49</v>
+      </c>
+      <c r="C806" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3">
+      <c r="A807" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B807" s="0">
+        <v>49</v>
+      </c>
+      <c r="C807" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3">
+      <c r="A808" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B808" s="0">
+        <v>49</v>
+      </c>
+      <c r="C808" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3">
+      <c r="A809" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B809" s="0">
+        <v>49</v>
+      </c>
+      <c r="C809" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3">
+      <c r="A810" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B810" s="0">
+        <v>49</v>
+      </c>
+      <c r="C810" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3">
+      <c r="A811" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B811" s="0">
+        <v>49</v>
+      </c>
+      <c r="C811" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3">
+      <c r="A812" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B812" s="0">
+        <v>49</v>
+      </c>
+      <c r="C812" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="813" spans="1:3">
+      <c r="A813" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B813" s="0">
+        <v>49</v>
+      </c>
+      <c r="C813" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3">
+      <c r="A814" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B814" s="0">
+        <v>49</v>
+      </c>
+      <c r="C814" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3">
+      <c r="A815" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B815" s="0">
+        <v>49</v>
+      </c>
+      <c r="C815" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3">
+      <c r="A816" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B816" s="0">
+        <v>49</v>
+      </c>
+      <c r="C816" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3">
+      <c r="A817" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B817" s="0">
+        <v>49</v>
+      </c>
+      <c r="C817" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3">
+      <c r="A818" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B818" s="0">
+        <v>49</v>
+      </c>
+      <c r="C818" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3">
+      <c r="A819" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B819" s="0">
+        <v>49</v>
+      </c>
+      <c r="C819" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3">
+      <c r="A820" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B820" s="0">
+        <v>49</v>
+      </c>
+      <c r="C820" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3">
+      <c r="A821" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B821" s="0">
+        <v>49</v>
+      </c>
+      <c r="C821" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3">
+      <c r="A822" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B822" s="0">
+        <v>49</v>
+      </c>
+      <c r="C822" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3">
+      <c r="A823" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B823" s="0">
+        <v>49</v>
+      </c>
+      <c r="C823" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3">
+      <c r="A824" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B824" s="0">
+        <v>49</v>
+      </c>
+      <c r="C824" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3">
+      <c r="A825" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B825" s="0">
+        <v>49</v>
+      </c>
+      <c r="C825" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3">
+      <c r="A826" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B826" s="0">
+        <v>49</v>
+      </c>
+      <c r="C826" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3">
+      <c r="A827" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B827" s="0">
+        <v>49</v>
+      </c>
+      <c r="C827" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="828" spans="1:3">
+      <c r="A828" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B828" s="0">
+        <v>49</v>
+      </c>
+      <c r="C828" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3">
+      <c r="A829" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B829" s="0">
+        <v>49</v>
+      </c>
+      <c r="C829" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3">
+      <c r="A830" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B830" s="0">
+        <v>49</v>
+      </c>
+      <c r="C830" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3">
+      <c r="A831" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B831" s="0">
+        <v>49</v>
+      </c>
+      <c r="C831" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3">
+      <c r="A832" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B832" s="0">
+        <v>49</v>
+      </c>
+      <c r="C832" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3">
+      <c r="A833" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B833" s="0">
+        <v>77</v>
+      </c>
+      <c r="C833" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3">
+      <c r="A834" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B834" s="0">
+        <v>77</v>
+      </c>
+      <c r="C834" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="835" spans="1:3">
+      <c r="A835" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B835" s="0">
+        <v>76</v>
+      </c>
+      <c r="C835" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="836" spans="1:3">
+      <c r="A836" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B836" s="0">
+        <v>49</v>
+      </c>
+      <c r="C836" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="837" spans="1:3">
+      <c r="A837" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B837" s="0">
+        <v>103</v>
+      </c>
+      <c r="C837" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="838" spans="1:3">
+      <c r="A838" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B838" s="0">
+        <v>103</v>
+      </c>
+      <c r="C838" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="839" spans="1:3">
+      <c r="A839" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B839" s="0">
+        <v>103</v>
+      </c>
+      <c r="C839" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="840" spans="1:3">
+      <c r="A840" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B840" s="0">
+        <v>86</v>
+      </c>
+      <c r="C840" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3">
+      <c r="A841" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B841" s="0">
+        <v>58</v>
+      </c>
+      <c r="C841" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="842" spans="1:3">
+      <c r="A842" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B842" s="0">
+        <v>64</v>
+      </c>
+      <c r="C842" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="843" spans="1:3">
+      <c r="A843" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B843" s="0">
+        <v>49</v>
+      </c>
+      <c r="C843" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="844" spans="1:3">
+      <c r="A844" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B844" s="0">
+        <v>144</v>
+      </c>
+      <c r="C844" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="845" spans="1:3">
+      <c r="A845" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B845" s="0">
+        <v>50</v>
+      </c>
+      <c r="C845" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="846" spans="1:3">
+      <c r="A846" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B846" s="0">
+        <v>103</v>
+      </c>
+      <c r="C846" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="847" spans="1:3">
+      <c r="A847" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B847" s="0">
+        <v>72</v>
+      </c>
+      <c r="C847" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="848" spans="1:3">
+      <c r="A848" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B848" s="0">
+        <v>56</v>
+      </c>
+      <c r="C848" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="849" spans="1:3">
+      <c r="A849" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B849" s="0">
+        <v>145</v>
+      </c>
+      <c r="C849" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="850" spans="1:3">
+      <c r="A850" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B850" s="0">
+        <v>139</v>
+      </c>
+      <c r="C850" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="851" spans="1:3">
+      <c r="A851" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B851" s="0">
+        <v>149</v>
+      </c>
+      <c r="C851" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="852" spans="1:3">
+      <c r="A852" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B852" s="0">
+        <v>153</v>
+      </c>
+      <c r="C852" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="853" spans="1:3">
+      <c r="A853" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B853" s="0">
+        <v>149</v>
+      </c>
+      <c r="C853" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="854" spans="1:3">
+      <c r="A854" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B854" s="0">
+        <v>144</v>
+      </c>
+      <c r="C854" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="855" spans="1:3">
+      <c r="A855" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B855" s="0">
+        <v>145</v>
+      </c>
+      <c r="C855" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="856" spans="1:3">
+      <c r="A856" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B856" s="0">
+        <v>73</v>
+      </c>
+      <c r="C856" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="857" spans="1:3">
+      <c r="A857" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B857" s="0">
+        <v>136</v>
+      </c>
+      <c r="C857" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="858" spans="1:3">
+      <c r="A858" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B858" s="0">
+        <v>145</v>
+      </c>
+      <c r="C858" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3">
+      <c r="A859" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B859" s="0">
+        <v>49</v>
+      </c>
+      <c r="C859" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="860" spans="1:3">
+      <c r="A860" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B860" s="0">
+        <v>49</v>
+      </c>
+      <c r="C860" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="861" spans="1:3">
+      <c r="A861" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B861" s="0">
+        <v>49</v>
+      </c>
+      <c r="C861" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="862" spans="1:3">
+      <c r="A862" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B862" s="0">
+        <v>49</v>
+      </c>
+      <c r="C862" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="863" spans="1:3">
+      <c r="A863" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B863" s="0">
+        <v>136</v>
+      </c>
+      <c r="C863" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="864" spans="1:3">
+      <c r="A864" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B864" s="0">
+        <v>71</v>
+      </c>
+      <c r="C864" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3">
+      <c r="A865" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B865" s="0">
+        <v>182</v>
+      </c>
+      <c r="C865" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3">
+      <c r="A866" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B866" s="0">
+        <v>50</v>
+      </c>
+      <c r="C866" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3">
+      <c r="A867" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B867" s="0">
+        <v>215</v>
+      </c>
+      <c r="C867" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3">
+      <c r="A868" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B868" s="0">
+        <v>144</v>
+      </c>
+      <c r="C868" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3">
+      <c r="A869" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B869" s="0">
+        <v>64</v>
+      </c>
+      <c r="C869" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="870" spans="1:3">
+      <c r="A870" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B870" s="0">
+        <v>145</v>
+      </c>
+      <c r="C870" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="871" spans="1:3">
+      <c r="A871" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B871" s="0">
+        <v>172</v>
+      </c>
+      <c r="C871" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="872" spans="1:3">
+      <c r="A872" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B872" s="0">
+        <v>169</v>
+      </c>
+      <c r="C872" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix dường dẫn python cho windown
</commit_message>
<xml_diff>
--- a/admin/pages/Association-Rules/dataset/viewlist.xlsx
+++ b/admin/pages/Association-Rules/dataset/viewlist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>ngayxem</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>2024-06-29</t>
+  </si>
+  <si>
+    <t>2024-06-30</t>
+  </si>
+  <si>
+    <t>2024-07-01</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C872"/>
+  <dimension ref="A1:C918"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -10038,6 +10044,512 @@
       </c>
       <c r="C872" s="0">
         <v>28</v>
+      </c>
+    </row>
+    <row r="873" spans="1:3">
+      <c r="A873" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B873" s="0">
+        <v>50</v>
+      </c>
+      <c r="C873" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="874" spans="1:3">
+      <c r="A874" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B874" s="0">
+        <v>91</v>
+      </c>
+      <c r="C874" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="875" spans="1:3">
+      <c r="A875" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B875" s="0">
+        <v>56</v>
+      </c>
+      <c r="C875" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="876" spans="1:3">
+      <c r="A876" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B876" s="0">
+        <v>75</v>
+      </c>
+      <c r="C876" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="877" spans="1:3">
+      <c r="A877" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B877" s="0">
+        <v>137</v>
+      </c>
+      <c r="C877" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="878" spans="1:3">
+      <c r="A878" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B878" s="0">
+        <v>138</v>
+      </c>
+      <c r="C878" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="879" spans="1:3">
+      <c r="A879" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B879" s="0">
+        <v>136</v>
+      </c>
+      <c r="C879" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="880" spans="1:3">
+      <c r="A880" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B880" s="0">
+        <v>139</v>
+      </c>
+      <c r="C880" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="881" spans="1:3">
+      <c r="A881" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B881" s="0">
+        <v>140</v>
+      </c>
+      <c r="C881" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="882" spans="1:3">
+      <c r="A882" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B882" s="0">
+        <v>141</v>
+      </c>
+      <c r="C882" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="883" spans="1:3">
+      <c r="A883" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B883" s="0">
+        <v>142</v>
+      </c>
+      <c r="C883" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="884" spans="1:3">
+      <c r="A884" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B884" s="0">
+        <v>143</v>
+      </c>
+      <c r="C884" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="885" spans="1:3">
+      <c r="A885" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B885" s="0">
+        <v>144</v>
+      </c>
+      <c r="C885" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="886" spans="1:3">
+      <c r="A886" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B886" s="0">
+        <v>145</v>
+      </c>
+      <c r="C886" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="887" spans="1:3">
+      <c r="A887" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B887" s="0">
+        <v>146</v>
+      </c>
+      <c r="C887" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="888" spans="1:3">
+      <c r="A888" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B888" s="0">
+        <v>147</v>
+      </c>
+      <c r="C888" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="889" spans="1:3">
+      <c r="A889" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B889" s="0">
+        <v>138</v>
+      </c>
+      <c r="C889" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="890" spans="1:3">
+      <c r="A890" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B890" s="0">
+        <v>49</v>
+      </c>
+      <c r="C890" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="891" spans="1:3">
+      <c r="A891" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B891" s="0">
+        <v>59</v>
+      </c>
+      <c r="C891" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="892" spans="1:3">
+      <c r="A892" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B892" s="0">
+        <v>58</v>
+      </c>
+      <c r="C892" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="893" spans="1:3">
+      <c r="A893" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B893" s="0">
+        <v>80</v>
+      </c>
+      <c r="C893" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="894" spans="1:3">
+      <c r="A894" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B894" s="0">
+        <v>136</v>
+      </c>
+      <c r="C894" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="895" spans="1:3">
+      <c r="A895" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B895" s="0">
+        <v>75</v>
+      </c>
+      <c r="C895" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="896" spans="1:3">
+      <c r="A896" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B896" s="0">
+        <v>64</v>
+      </c>
+      <c r="C896" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="897" spans="1:3">
+      <c r="A897" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B897" s="0">
+        <v>138</v>
+      </c>
+      <c r="C897" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="898" spans="1:3">
+      <c r="A898" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B898" s="0">
+        <v>137</v>
+      </c>
+      <c r="C898" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="899" spans="1:3">
+      <c r="A899" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B899" s="0">
+        <v>182</v>
+      </c>
+      <c r="C899" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3">
+      <c r="A900" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B900" s="0">
+        <v>147</v>
+      </c>
+      <c r="C900" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="901" spans="1:3">
+      <c r="A901" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B901" s="0">
+        <v>167</v>
+      </c>
+      <c r="C901" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="902" spans="1:3">
+      <c r="A902" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B902" s="0">
+        <v>174</v>
+      </c>
+      <c r="C902" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="903" spans="1:3">
+      <c r="A903" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B903" s="0">
+        <v>226</v>
+      </c>
+      <c r="C903" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3">
+      <c r="A904" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B904" s="0">
+        <v>227</v>
+      </c>
+      <c r="C904" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="905" spans="1:3">
+      <c r="A905" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B905" s="0">
+        <v>58</v>
+      </c>
+      <c r="C905" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3">
+      <c r="A906" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B906" s="0">
+        <v>207</v>
+      </c>
+      <c r="C906" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="907" spans="1:3">
+      <c r="A907" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B907" s="0">
+        <v>139</v>
+      </c>
+      <c r="C907" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3">
+      <c r="A908" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B908" s="0">
+        <v>139</v>
+      </c>
+      <c r="C908" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="909" spans="1:3">
+      <c r="A909" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B909" s="0">
+        <v>55</v>
+      </c>
+      <c r="C909" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="910" spans="1:3">
+      <c r="A910" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B910" s="0">
+        <v>49</v>
+      </c>
+      <c r="C910" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="911" spans="1:3">
+      <c r="A911" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B911" s="0">
+        <v>212</v>
+      </c>
+      <c r="C911" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="912" spans="1:3">
+      <c r="A912" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B912" s="0">
+        <v>192</v>
+      </c>
+      <c r="C912" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="913" spans="1:3">
+      <c r="A913" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B913" s="0">
+        <v>49</v>
+      </c>
+      <c r="C913" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="914" spans="1:3">
+      <c r="A914" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B914" s="0">
+        <v>192</v>
+      </c>
+      <c r="C914" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="915" spans="1:3">
+      <c r="A915" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B915" s="0">
+        <v>62</v>
+      </c>
+      <c r="C915" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="916" spans="1:3">
+      <c r="A916" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B916" s="0">
+        <v>89</v>
+      </c>
+      <c r="C916" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="917" spans="1:3">
+      <c r="A917" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B917" s="0">
+        <v>228</v>
+      </c>
+      <c r="C917" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="918" spans="1:3">
+      <c r="A918" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B918" s="0">
+        <v>192</v>
+      </c>
+      <c r="C918" s="0">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>